<commit_message>
update files, to be deleted in future
</commit_message>
<xml_diff>
--- a/000_final_results/group_fam/results_summary_group_fam_back_projection.xlsx
+++ b/000_final_results/group_fam/results_summary_group_fam_back_projection.xlsx
@@ -528,20 +528,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373, 0.7373737373737373]</t>
+          <t>[0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1351.864252294801), np.float64(1349.93577261963), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1363.435130345826), np.float64(1348.007292944459), np.float64(1365.363610020997), np.float64(1346.078813269288), np.float64(1344.150333594117), np.float64(1367.292089696168), np.float64(1342.221853918946), np.float64(1340.293374243775), np.float64(1604.495089742189), np.float64(1369.220569371339), np.float64(1338.364894568605)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1351.864252294801), np.float64(1353.792731969972), np.float64(1349.93577261963), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1348.007292944459), np.float64(1363.435130345826), np.float64(1346.078813269288), np.float64(1365.363610020997), np.float64(1604.495089742189), np.float64(1344.150333594117), np.float64(1170.587162828736), np.float64(1168.658683153565), np.float64(1367.292089696168), np.float64(1342.221853918946), np.float64(1172.515642503907)]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.00746222 0.00520422 0.00442044 0.00437769 0.00437616 0.00435722
- 0.00434978 0.00434613 0.00434119 0.0042533  0.00422022 0.00405084
- 0.00404433 0.00386953 0.00382619 0.00376447 0.003731   0.00369776
- 0.00365549 0.00364043]</t>
+          <t>[0.0074686  0.00522313 0.00415454 0.00412119 0.00411308 0.00409827
+ 0.00408069 0.00406691 0.00405336 0.00397873 0.00396621 0.00382488
+ 0.00378309 0.00370876 0.00366888 0.00364508 0.00363191 0.0035924
+ 0.00356379 0.00355674]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -608,20 +608,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743, 0.7744107744107743]</t>
+          <t>[0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046, 0.8047138047138046]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1351.864252294801), np.float64(1349.93577261963), np.float64(1353.792731969972), np.float64(1348.007292944459), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1346.078813269288), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1344.150333594117), np.float64(1363.435130345826), np.float64(1342.221853918946), np.float64(1365.363610020997), np.float64(1340.293374243775), np.float64(1338.364894568605), np.float64(1367.292089696168), np.float64(1336.436414893434), np.float64(1369.220569371339)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1349.93577261963), np.float64(1351.864252294801), np.float64(1348.007292944459), np.float64(1346.078813269288), np.float64(1344.150333594117), np.float64(1353.792731969972), np.float64(1342.221853918946), np.float64(1340.293374243775), np.float64(1355.721211645143), np.float64(1338.364894568605), np.float64(1357.649691320314), np.float64(1361.506650670656), np.float64(1359.578170995484), np.float64(1336.436414893434), np.float64(1363.435130345826), np.float64(952.6689595344246), np.float64(1365.363610020997), np.float64(1334.507935218263)]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0.00447413 0.00374818 0.00344597 0.00344044 0.00341631 0.00340104
- 0.00338239 0.0033507  0.00334727 0.00332596 0.00331042 0.00327456
- 0.0032602  0.00320512 0.00316572 0.00314838 0.00307972 0.00307925
- 0.00300499 0.00300426]</t>
+          <t>[0.00394785 0.00357629 0.00287796 0.00286729 0.00286695 0.00285643
+ 0.00283577 0.00282879 0.00282507 0.00282133 0.00279502 0.00278933
+ 0.00276845 0.00276581 0.00275696 0.00274678 0.00274459 0.00272428
+ 0.00269118 0.00267607]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -688,20 +688,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685, 0.8183501683501685]</t>
+          <t>[0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609, 0.7609427609427609]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1604.495089742189), np.float64(1598.709650716676), np.float64(1170.587162828736), np.float64(1172.515642503907), np.float64(1168.658683153565), np.float64(1641.136203570436), np.float64(1643.064683245607), np.float64(1174.444122179078), np.float64(1166.730203478395), np.float64(1639.207723895265), np.float64(1702.847553175905), np.float64(1704.776032851076), np.float64(1176.372601854249), np.float64(948.812000184083), np.float64(1164.801723803224), np.float64(1178.30108152942), np.float64(1700.919073500734), np.float64(1349.93577261963)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1604.495089742189), np.float64(1641.136203570436), np.float64(1643.064683245607), np.float64(1639.207723895265), np.float64(1598.709650716676), np.float64(1170.587162828736), np.float64(1168.658683153565), np.float64(1172.515642503907), np.float64(1166.730203478395), np.float64(950.7404798592538), np.float64(1637.279244220094), np.float64(1174.444122179078), np.float64(1164.801723803224), np.float64(952.6689595344246), np.float64(2927.432146909426), np.float64(2929.360626584597), np.float64(948.812000184083), np.float64(2925.503667234255)]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[0.00742836 0.00535939 0.00353259 0.00346497 0.00331703 0.00331477
- 0.00323141 0.0032042  0.00315453 0.00313082 0.00308587 0.0030378
- 0.00294425 0.00294308 0.00293295 0.00286658 0.00279861 0.0026538
- 0.00260569 0.0026032 ]</t>
+          <t>[0.01054876 0.00713857 0.00544944 0.00498559 0.00459656 0.00451723
+ 0.00435044 0.00402282 0.00396345 0.0039196  0.00378561 0.00368401
+ 0.00364961 0.00354929 0.00350765 0.00342004 0.00341778 0.00340576
+ 0.00337701 0.00334273]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -773,15 +773,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1604.495089742189), np.float64(3048.926366445193), np.float64(1351.864252294801), np.float64(1353.792731969972), np.float64(1349.93577261963), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1348.007292944459), np.float64(1363.435130345826), np.float64(1346.078813269288), np.float64(1365.363610020997), np.float64(1344.150333594117), np.float64(1367.292089696168), np.float64(1342.221853918946), np.float64(1704.776032851076), np.float64(1340.293374243775)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1604.495089742189), np.float64(1351.864252294801), np.float64(1349.93577261963), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1348.007292944459), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1346.078813269288), np.float64(1363.435130345826), np.float64(1170.587162828736), np.float64(1168.658683153565), np.float64(1344.150333594117), np.float64(1172.515642503907), np.float64(1365.363610020997), np.float64(1166.730203478395), np.float64(1342.221853918946)]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[0.00960718 0.00617239 0.0052302  0.00519521 0.00514722 0.00511137
- 0.00507923 0.00506533 0.00501761 0.00496782 0.00491196 0.00488434
- 0.00476936 0.00464134 0.00450293 0.00438464 0.00422149 0.00417852
- 0.00405806 0.00404261]</t>
+          <t>[0.00988068 0.0065105  0.00524529 0.00480018 0.0047672  0.00472877
+ 0.00466439 0.00461066 0.00460929 0.00456947 0.00453771 0.00442
+ 0.0044165  0.00432853 0.00431059 0.0042247  0.0041919  0.004177
+ 0.00413597 0.00409296]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -848,20 +848,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973, 0.7737556561085973]</t>
+          <t>[0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229, 0.7993966817496229]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1643.064683245607), np.float64(1641.136203570436), np.float64(3048.926366445193), np.float64(1706.704512526246), np.float64(1600.638130391847), np.float64(1644.993162920778), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1159.016284777711), np.float64(1357.649691320314), np.float64(1351.864252294801), np.float64(1359.578170995484), np.float64(1160.944764452882), np.float64(1349.93577261963), np.float64(1164.801723803224), np.float64(1704.776032851076), np.float64(1162.873244128053), np.float64(1361.506650670656), np.float64(1348.007292944459)]</t>
+          <t>[np.float64(1643.064683245607), np.float64(1602.566610067018), np.float64(1641.136203570436), np.float64(3048.926366445193), np.float64(1706.704512526246), np.float64(1644.993162920778), np.float64(1600.638130391847), np.float64(1159.016284777711), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1351.864252294801), np.float64(1160.944764452882), np.float64(1164.801723803224), np.float64(1162.873244128053), np.float64(1359.578170995484), np.float64(1361.506650670656), np.float64(1349.93577261963), np.float64(1168.658683153565), np.float64(1170.587162828736)]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[0.00535818 0.00527303 0.00501336 0.00494027 0.00422045 0.00402648
- 0.00397207 0.00364124 0.00360306 0.0035769  0.00351563 0.00350929
- 0.00344659 0.0033885  0.00337766 0.00337177 0.00337106 0.00337
- 0.00335314 0.00331397]</t>
+          <t>[0.00527864 0.00522942 0.00498432 0.00450891 0.00408998 0.00400178
+ 0.00394978 0.00363087 0.00359941 0.00356911 0.00349027 0.00346685
+ 0.00345187 0.00343393 0.00343235 0.00342811 0.00334182 0.00333551
+ 0.00333472 0.00332754]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1008,20 +1008,20 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875, 0.7345399698340875]</t>
+          <t>[0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619, 0.7088989441930619]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1643.064683245607), np.float64(1600.638130391847), np.float64(1641.136203570436), np.float64(954.5974392095954), np.float64(956.5259188847667), np.float64(952.6689595344246), np.float64(1644.993162920778), np.float64(950.7404798592538), np.float64(1216.870675032838), np.float64(1214.942195357667), np.float64(1220.72763438318), np.float64(1218.799154708009), np.float64(958.4543985599371), np.float64(1213.013715682496), np.float64(1222.656114058351), np.float64(944.9550408337414), np.float64(1211.085236007325), np.float64(946.8835205089117), np.float64(1170.587162828736)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(954.5974392095954), np.float64(1643.064683245607), np.float64(956.5259188847667), np.float64(952.6689595344246), np.float64(1641.136203570436), np.float64(1600.638130391847), np.float64(950.7404798592538), np.float64(1216.870675032838), np.float64(1220.72763438318), np.float64(1214.942195357667), np.float64(958.4543985599371), np.float64(1218.799154708009), np.float64(1644.993162920778), np.float64(1222.656114058351), np.float64(1213.013715682496), np.float64(1211.085236007325), np.float64(944.9550408337414), np.float64(962.3113579102792), np.float64(1159.016284777711)]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[0.00420249 0.00386642 0.003581   0.00352801 0.00352081 0.00341524
- 0.00338409 0.00304086 0.00298214 0.00291605 0.00288108 0.00285749
- 0.00285172 0.00285064 0.00278945 0.00268943 0.00267769 0.00267442
- 0.0026073  0.00258996]</t>
+          <t>[0.0041256  0.00402913 0.00394378 0.0038873  0.00383269 0.00357386
+ 0.00356187 0.00327835 0.00319597 0.00318849 0.00316574 0.00313377
+ 0.00311857 0.00310563 0.00310376 0.00306443 0.00292859 0.00287962
+ 0.00284171 0.00276562]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1093,15 +1093,15 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(3048.926366445193), np.float64(1706.704512526246), np.float64(1641.136203570436), np.float64(1643.064683245607), np.float64(1708.632992201417), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1704.776032851076), np.float64(1359.578170995484), np.float64(1600.638130391847), np.float64(1351.864252294801), np.float64(1361.506650670656), np.float64(1349.93577261963), np.float64(1363.435130345826), np.float64(1348.007292944459), np.float64(1365.363610020997), np.float64(1346.078813269288), np.float64(1367.292089696168)]</t>
+          <t>[np.float64(3048.926366445193), np.float64(1602.566610067018), np.float64(1641.136203570436), np.float64(1643.064683245607), np.float64(1706.704512526246), np.float64(1600.638130391847), np.float64(1708.632992201417), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1704.776032851076), np.float64(1357.649691320314), np.float64(1351.864252294801), np.float64(1359.578170995484), np.float64(1349.93577261963), np.float64(1361.506650670656), np.float64(1348.007292944459), np.float64(1363.435130345826), np.float64(1604.495089742189), np.float64(1644.993162920778), np.float64(1346.078813269288)]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[0.00677091 0.00599409 0.00580133 0.00575828 0.0056974  0.00496379
- 0.00483283 0.00482125 0.00473108 0.00468106 0.00464869 0.00463046
- 0.00462055 0.00451415 0.00440391 0.00434621 0.00426306 0.00418912
- 0.00407482 0.00407068]</t>
+          <t>[0.00892993 0.00757654 0.00568876 0.00559648 0.00547229 0.00507
+ 0.00480227 0.00460291 0.00454929 0.00445865 0.0044242  0.00442346
+ 0.0043175  0.00423171 0.00416915 0.00410501 0.00400137 0.00399865
+ 0.00396894 0.00391934]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1168,20 +1168,20 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517, 0.7809036658141517]</t>
+          <t>[0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615, 0.8201193520886615]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[np.float64(3048.926366445193), np.float64(1602.566610067018), np.float64(1643.064683245607), np.float64(1706.704512526246), np.float64(1641.136203570436), np.float64(1737.560187328981), np.float64(1353.792731969972), np.float64(1600.638130391847), np.float64(1735.63170765381), np.float64(1355.721211645143), np.float64(1159.016284777711), np.float64(1720.203870252443), np.float64(1644.993162920778), np.float64(1351.864252294801), np.float64(1704.776032851076), np.float64(1357.649691320314), np.float64(1731.774748303468), np.float64(1359.578170995484), np.float64(1739.488667004152), np.float64(1733.703227978639)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(3048.926366445193), np.float64(1643.064683245607), np.float64(1641.136203570436), np.float64(1706.704512526246), np.float64(1600.638130391847), np.float64(1644.993162920778), np.float64(1159.016284777711), np.float64(1737.560187328981), np.float64(1353.792731969972), np.float64(1735.63170765381), np.float64(1720.203870252443), np.float64(1355.721211645143), np.float64(1160.944764452882), np.float64(1164.801723803224), np.float64(1351.864252294801), np.float64(1162.873244128053), np.float64(1704.776032851076), np.float64(1357.649691320314), np.float64(1731.774748303468)]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[0.00598392 0.00508835 0.00464894 0.0045282  0.00449106 0.00386496
- 0.00376991 0.00376421 0.00372844 0.00370755 0.00366255 0.00366024
- 0.00364872 0.00364203 0.00361605 0.00361367 0.00356578 0.0035448
- 0.00353914 0.00350269]</t>
+          <t>[0.00547404 0.00538434 0.00494534 0.00493682 0.00425902 0.0040834
+ 0.00372957 0.00369984 0.00367624 0.00355677 0.00353419 0.00352691
+ 0.0034884  0.00346379 0.00345638 0.00344483 0.0034312  0.0034222
+ 0.00339331 0.00338616]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1248,20 +1248,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165, 0.8397271952259165]</t>
+          <t>[0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714, 0.8593350383631714]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1353.792731969972), np.float64(1351.864252294801), np.float64(1355.721211645143), np.float64(1349.93577261963), np.float64(1357.649691320314), np.float64(1348.007292944459), np.float64(1359.578170995484), np.float64(1346.078813269288), np.float64(1361.506650670656), np.float64(1344.150333594117), np.float64(1363.435130345826), np.float64(1342.221853918946), np.float64(1365.363610020997), np.float64(1706.704512526246), np.float64(1367.292089696168), np.float64(2927.432146909426), np.float64(2929.360626584597), np.float64(1369.220569371339)]</t>
+          <t>[np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1351.864252294801), np.float64(1357.649691320314), np.float64(1359.578170995484), np.float64(1349.93577261963), np.float64(1361.506650670656), np.float64(1348.007292944459), np.float64(1363.435130345826), np.float64(1346.078813269288), np.float64(1365.363610020997), np.float64(1344.150333594117), np.float64(1367.292089696168), np.float64(1342.221853918946), np.float64(1369.220569371339), np.float64(1340.293374243775), np.float64(1602.566610067018), np.float64(1371.14904904651), np.float64(1338.364894568605), np.float64(1600.638130391847)]</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[0.00296132 0.00283094 0.00269865 0.00267504 0.0026669  0.0026397
- 0.00263205 0.00262934 0.00261321 0.00260269 0.00259008 0.00256875
- 0.00255572 0.00252758 0.00252029 0.00251977 0.00250033 0.00247591
- 0.00246076 0.00245463]</t>
+          <t>[0.00313395 0.00311664 0.00310247 0.00309201 0.00307649 0.00305443
+ 0.00305307 0.003015   0.00301093 0.00295629 0.00294804 0.00288768
+ 0.00288154 0.00281102 0.0027947  0.00271512 0.00268066 0.00266187
+ 0.00263066 0.00261585]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1328,20 +1328,20 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901, 0.6990403742321901]</t>
+          <t>[0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334, 0.7331409709926334]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[np.float64(3048.926366445193), np.float64(1159.016284777711), np.float64(1222.656114058351), np.float64(1353.792731969972), np.float64(1157.08780510254), np.float64(1355.721211645143), np.float64(1160.944764452882), np.float64(1357.649691320314), np.float64(1351.864252294801), np.float64(1643.064683245607), np.float64(1359.578170995484), np.float64(1706.704512526246), np.float64(1737.560187328981), np.float64(1162.873244128053), np.float64(1361.506650670656), np.float64(1213.013715682496), np.float64(1720.203870252443), np.float64(1164.801723803224), np.float64(1349.93577261963), np.float64(1224.584593733522)]</t>
+          <t>[np.float64(3048.926366445193), np.float64(1159.016284777711), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1357.649691320314), np.float64(1359.578170995484), np.float64(1351.864252294801), np.float64(1706.704512526246), np.float64(1361.506650670656), np.float64(1157.08780510254), np.float64(1222.656114058351), np.float64(1737.560187328981), np.float64(1160.944764452882), np.float64(1349.93577261963), np.float64(1720.203870252443), np.float64(1363.435130345826), np.float64(1643.064683245607), np.float64(1348.007292944459), np.float64(1365.363610020997), np.float64(1213.013715682496)]</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[0.00464531 0.00458439 0.00423636 0.00423452 0.0042255  0.00418423
- 0.00411447 0.00408768 0.00403941 0.00402601 0.00402106 0.00401536
- 0.00396145 0.00390893 0.00390428 0.00385793 0.00385419 0.00382608
- 0.00381777 0.00381424]</t>
+          <t>[0.00504751 0.004326   0.00429604 0.00426019 0.00417566 0.00411339
+ 0.00409842 0.00403729 0.00399466 0.00399082 0.00399073 0.00390557
+ 0.0038842  0.00387445 0.00386926 0.00385359 0.0037934  0.00375767
+ 0.00375586 0.00372722]</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1408,20 +1408,20 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067, 0.8005115089514067]</t>
+          <t>[0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835, 0.8294970161977835]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[np.float64(3048.926366445193), np.float64(1706.704512526246), np.float64(1602.566610067018), np.float64(1641.136203570436), np.float64(3046.997886770022), np.float64(1643.064683245607), np.float64(1737.560187328981), np.float64(1708.632992201417), np.float64(1735.63170765381), np.float64(1704.776032851076), np.float64(1720.203870252443), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1731.774748303468), np.float64(1351.864252294801), np.float64(1733.703227978639), np.float64(1739.488667004152), np.float64(1357.649691320314), np.float64(1718.275390577272), np.float64(1008.594870114381)]</t>
+          <t>[np.float64(3048.926366445193), np.float64(1641.136203570436), np.float64(1643.064683245607), np.float64(1602.566610067018), np.float64(1706.704512526246), np.float64(1353.792731969972), np.float64(1355.721211645143), np.float64(1644.993162920778), np.float64(1737.560187328981), np.float64(1357.649691320314), np.float64(1351.864252294801), np.float64(1159.016284777711), np.float64(1359.578170995484), np.float64(1735.63170765381), np.float64(1720.203870252443), np.float64(1164.801723803224), np.float64(1170.587162828736), np.float64(1361.506650670656), np.float64(1168.658683153565), np.float64(1162.873244128053)]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[0.01110082 0.0059547  0.00554886 0.00519667 0.00506411 0.00501306
- 0.00472056 0.00467487 0.00455713 0.00453775 0.00451233 0.00444772
- 0.00435472 0.00429154 0.00425045 0.0042267  0.00421467 0.00420884
- 0.00413482 0.00411197]</t>
+          <t>[0.0064592  0.00587945 0.00581034 0.00575942 0.00493128 0.00438998
+ 0.00433836 0.00432676 0.00431418 0.0042436  0.00422162 0.00420802
+ 0.00417019 0.00416949 0.00412035 0.00410185 0.00404383 0.00403396
+ 0.00403194 0.00401182]</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1488,20 +1488,20 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091, 0.8090909090909091]</t>
+          <t>[0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394, 0.793939393939394]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[np.float64(1105.018853872926), np.float64(1106.947333548097), np.float64(1103.090374197755), np.float64(1108.875813223267), np.float64(968.0967969357921), np.float64(966.1683172606208), np.float64(970.0252766109629), np.float64(1101.161894522584), np.float64(964.23983758545), np.float64(971.9537562861337), np.float64(1110.804292898438), np.float64(939.1696018082284), np.float64(962.3113579102792), np.float64(950.7404798592538), np.float64(941.0980814833993), np.float64(952.6689595344246), np.float64(973.8822359613046), np.float64(948.812000184083), np.float64(960.3828782351084), np.float64(954.5974392095954)]</t>
+          <t>[np.float64(1105.018853872926), np.float64(1106.947333548097), np.float64(1103.090374197755), np.float64(1108.875813223267), np.float64(968.0967969357921), np.float64(970.0252766109629), np.float64(966.1683172606208), np.float64(1101.161894522584), np.float64(964.23983758545), np.float64(971.9537562861337), np.float64(939.1696018082284), np.float64(1110.804292898438), np.float64(962.3113579102792), np.float64(941.0980814833993), np.float64(950.7404798592538), np.float64(952.6689595344246), np.float64(973.8822359613046), np.float64(948.812000184083), np.float64(960.3828782351084), np.float64(954.5974392095954)]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[0.00387378 0.00382165 0.00377723 0.00368094 0.00362388 0.00360181
- 0.00360139 0.00354095 0.0035352  0.0034966  0.00348391 0.0034636
- 0.0034186  0.00340971 0.00340497 0.00339611 0.00337099 0.00335032
- 0.00334663 0.00333898]</t>
+          <t>[0.00383765 0.00377074 0.00375817 0.00361875 0.00356797 0.00354602
+ 0.0035453  0.00354061 0.00347669 0.0034376  0.00341375 0.00341268
+ 0.00335419 0.0033463  0.00334141 0.00332497 0.00330565 0.00328165
+ 0.00327779 0.00326446]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1568,20 +1568,20 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303]</t>
+          <t>[0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727, 0.8727272727272727]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[np.float64(1554.354618187745), np.float64(1552.426138512574), np.float64(1556.283097862916), np.float64(1010.523349789552), np.float64(1008.594870114381), np.float64(1012.451829464723), np.float64(1550.497658837404), np.float64(1006.66639043921), np.float64(1004.737910764039), np.float64(1014.380309139893), np.float64(1548.569179162233), np.float64(1016.308788815064), np.float64(1002.809431088868), np.float64(1546.640699487062), np.float64(1558.211577538087), np.float64(1544.712219811891), np.float64(1000.880951413697), np.float64(968.0967969357921), np.float64(1018.237268490235), np.float64(1542.78374013672)]</t>
+          <t>[np.float64(1554.354618187745), np.float64(1556.283097862916), np.float64(1552.426138512574), np.float64(1010.523349789552), np.float64(1012.451829464723), np.float64(1008.594870114381), np.float64(1558.211577538087), np.float64(1014.380309139893), np.float64(1006.66639043921), np.float64(1550.497658837404), np.float64(1016.308788815064), np.float64(1644.993162920778), np.float64(1004.737910764039), np.float64(1018.237268490235), np.float64(1002.809431088868), np.float64(1646.921642595948), np.float64(1548.569179162233), np.float64(1000.880951413697), np.float64(1546.640699487062), np.float64(1560.140057213258)]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[0.00366521 0.00359147 0.00358179 0.00349913 0.00349218 0.00347172
- 0.00346721 0.00346521 0.0033928  0.00339274 0.00335973 0.003302
- 0.00329827 0.00328017 0.00327124 0.0032263  0.003185   0.00318391
- 0.00317968 0.00317671]</t>
+          <t>[0.00371641 0.00371075 0.0035474  0.00348954 0.00348791 0.00346684
+ 0.00346156 0.00344058 0.00343647 0.00339256 0.003385   0.00337036
+ 0.00336947 0.00329197 0.00328492 0.00326361 0.0032569  0.00318256
+ 0.00314358 0.00313736]</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1648,20 +1648,20 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545, 0.6545454545454545]</t>
+          <t>[0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333, 0.7333333333333333]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[np.float64(1716.346910902101), np.float64(1683.562756424196), np.float64(1681.634276749025), np.float64(1685.491236099367), np.float64(1679.705797073854), np.float64(1552.426138512574), np.float64(1554.354618187745), np.float64(1008.594870114381), np.float64(1006.66639043921), np.float64(1550.497658837404), np.float64(1010.523349789552), np.float64(1548.569179162233), np.float64(1546.640699487062), np.float64(970.0252766109629), np.float64(1544.712219811891), np.float64(1542.78374013672), np.float64(1004.737910764039), np.float64(1677.777317398683), np.float64(1012.451829464723), np.float64(1556.283097862916)]</t>
+          <t>[np.float64(1716.346910902101), np.float64(1006.66639043921), np.float64(970.0252766109629), np.float64(1008.594870114381), np.float64(968.0967969357921), np.float64(1010.523349789552), np.float64(966.1683172606208), np.float64(1004.737910764039), np.float64(971.9537562861337), np.float64(1012.451829464723), np.float64(964.23983758545), np.float64(1552.426138512574), np.float64(1683.562756424196), np.float64(1014.380309139893), np.float64(1681.634276749025), np.float64(1554.354618187745), np.float64(1002.809431088868), np.float64(1016.308788815064), np.float64(1550.497658837404), np.float64(973.8822359613046)]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[0.00360731 0.00351457 0.00349549 0.00342672 0.00338216 0.00337873
- 0.00335645 0.00331391 0.00331089 0.0033068  0.00326697 0.00325643
- 0.00324687 0.00323741 0.00322527 0.00322203 0.00321757 0.00320376
- 0.00320176 0.00320107]</t>
+          <t>[0.00331375 0.00317398 0.00317264 0.00316964 0.00315129 0.00312761
+ 0.00308564 0.00307563 0.00307229 0.0030698  0.00298943 0.00298196
+ 0.00297659 0.00297611 0.00296867 0.00295258 0.00292207 0.00291332
+ 0.00290299 0.00289573]</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1728,20 +1728,20 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696, 0.8696969696969696]</t>
+          <t>[0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303, 0.903030303030303]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[np.float64(1105.018853872926), np.float64(1106.947333548097), np.float64(1103.090374197755), np.float64(1108.875813223267), np.float64(966.1683172606208), np.float64(968.0967969357921), np.float64(964.23983758545), np.float64(970.0252766109629), np.float64(1110.804292898438), np.float64(939.1696018082284), np.float64(971.9537562861337), np.float64(941.0980814833993), np.float64(962.3113579102792), np.float64(1101.161894522584), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(960.3828782351084), np.float64(958.4543985599371), np.float64(973.8822359613046)]</t>
+          <t>[np.float64(970.0252766109629), np.float64(968.0967969357921), np.float64(966.1683172606208), np.float64(971.9537562861337), np.float64(1105.018853872926), np.float64(1716.346910902101), np.float64(1106.947333548097), np.float64(964.23983758545), np.float64(1546.640699487062), np.float64(1103.090374197755), np.float64(973.8822359613046), np.float64(1548.569179162233), np.float64(1550.497658837404), np.float64(1544.712219811891), np.float64(1552.426138512574), np.float64(1108.875813223267), np.float64(1542.78374013672), np.float64(939.1696018082284), np.float64(1685.491236099367), np.float64(962.3113579102792)]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[0.00409616 0.00406036 0.00386252 0.003823   0.00355362 0.00353748
- 0.00352133 0.00351092 0.0034557  0.00344689 0.00341381 0.00341279
- 0.00340218 0.00339677 0.00337853 0.00336007 0.00332838 0.0033228
- 0.00330761 0.00330473]</t>
+          <t>[0.00355303 0.00352185 0.00346553 0.00346543 0.0034255  0.00342534
+ 0.00337958 0.00337195 0.00333689 0.00333559 0.00330878 0.00330207
+ 0.00328631 0.0032858  0.00327512 0.00325388 0.0032366  0.0032349
+ 0.00322867 0.00320238]</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1808,20 +1808,20 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924, 0.7983193277310924]</t>
+          <t>[0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395, 0.865546218487395]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[np.float64(1110.804292898438), np.float64(1112.732772573609), np.float64(1132.017569325318), np.float64(1108.875813223267), np.float64(1039.450544917115), np.float64(1130.089089650148), np.float64(1037.522065241944), np.float64(1041.379024592286), np.float64(1114.66125224878), np.float64(1035.593585566773), np.float64(1128.160609974977), np.float64(1133.946049000489), np.float64(1043.307504267457), np.float64(1126.232130299806), np.float64(1106.947333548097), np.float64(1116.589731923951), np.float64(1033.665105891602), np.float64(1124.303650624635), np.float64(1118.518211599122), np.float64(1122.375170949464)]</t>
+          <t>[np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1128.160609974977), np.float64(1126.232130299806), np.float64(1133.946049000489), np.float64(1112.732772573609), np.float64(1110.804292898438), np.float64(1114.66125224878), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1116.589731923951), np.float64(1108.875813223267), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1135.87452867566), np.float64(1039.450544917115), np.float64(1106.947333548097), np.float64(1041.379024592286), np.float64(1037.522065241944), np.float64(1035.593585566773)]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0.00383885 0.00381778 0.00379426 0.00378788 0.00378556 0.00377611
- 0.00376516 0.00375744 0.00373628 0.00371967 0.00371822 0.00370772
- 0.00365986 0.0036513  0.00364789 0.00361843 0.00361696 0.00357782
- 0.0035296  0.00352567]</t>
+          <t>[0.00400788 0.00399874 0.00396482 0.00390264 0.00387076 0.00387013
+ 0.00384502 0.00383274 0.00382454 0.00375697 0.00375576 0.00375354
+ 0.00371284 0.00370437 0.00362475 0.00359165 0.00358525 0.00357084
+ 0.00355792 0.00349635]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1893,15 +1893,15 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1130.089089650148), np.float64(1122.375170949464), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1133.946049000489), np.float64(1556.283097862916), np.float64(1558.211577538087), np.float64(1118.518211599122), np.float64(1554.354618187745), np.float64(1560.140057213258), np.float64(1673.920358048341), np.float64(1116.589731923951), np.float64(1675.848837723512), np.float64(1677.777317398683), np.float64(1135.87452867566), np.float64(1562.068536888429), np.float64(1671.99187837317)]</t>
+          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1130.089089650148), np.float64(1122.375170949464), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1556.283097862916), np.float64(1133.946049000489), np.float64(1558.211577538087), np.float64(1554.354618187745), np.float64(1118.518211599122), np.float64(1560.140057213258), np.float64(1673.920358048341), np.float64(1677.777317398683), np.float64(1675.848837723512), np.float64(1116.589731923951), np.float64(1679.705797073854), np.float64(1671.99187837317), np.float64(1135.87452867566)]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.00551333 0.00547772 0.00540306 0.00533559 0.00514197 0.00505192
- 0.00478446 0.00454358 0.00454289 0.0044559  0.00438541 0.00427313
- 0.00426716 0.00398435 0.00397559 0.00391747 0.00390337 0.00383862
- 0.00383212 0.0038034 ]</t>
+          <t>[0.00537891 0.00535163 0.00525138 0.00521052 0.00497353 0.00492253
+ 0.0046073  0.00447636 0.00440995 0.00435404 0.00424835 0.00420983
+ 0.00413905 0.00392885 0.00390325 0.00389245 0.00381926 0.00380265
+ 0.00372085 0.00371081]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2048,20 +2048,20 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737, 0.9089635854341737]</t>
+          <t>[0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974, 0.9327731092436974]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[np.float64(1110.804292898438), np.float64(1108.875813223267), np.float64(1039.450544917115), np.float64(1037.522065241944), np.float64(1112.732772573609), np.float64(1041.379024592286), np.float64(1035.593585566773), np.float64(1106.947333548097), np.float64(1043.307504267457), np.float64(1114.66125224878), np.float64(1033.665105891602), np.float64(1132.017569325318), np.float64(1130.089089650148), np.float64(1133.946049000489), np.float64(1045.235983942628), np.float64(1496.500227932618), np.float64(1116.589731923951), np.float64(1128.160609974977), np.float64(1031.736626216432), np.float64(1498.428707607789)]</t>
+          <t>[np.float64(1257.368748211427), np.float64(1039.450544917115), np.float64(1259.297227886598), np.float64(1037.522065241944), np.float64(1041.379024592286), np.float64(1035.593585566773), np.float64(1255.440268536256), np.float64(1043.307504267457), np.float64(1033.665105891602), np.float64(1496.500227932618), np.float64(1498.428707607789), np.float64(1130.089089650148), np.float64(1502.285666958131), np.float64(1128.160609974977), np.float64(1132.017569325318), np.float64(1500.35718728296), np.float64(1045.235983942628), np.float64(1556.283097862916), np.float64(1110.804292898438), np.float64(1126.232130299806)]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.00349527 0.00347391 0.00345784 0.00345256 0.00344314 0.00342744
- 0.00342505 0.00334803 0.00334412 0.0033353  0.00333298 0.00331494
- 0.00326986 0.00326868 0.0032316  0.00320805 0.00319885 0.00319624
- 0.00315678 0.0031539 ]</t>
+          <t>[0.00349683 0.00344042 0.00343628 0.00342088 0.00340989 0.00337643
+ 0.00331493 0.00330886 0.00327457 0.00323476 0.00323153 0.00321363
+ 0.00320309 0.00319291 0.00319195 0.00317058 0.0031651  0.00316468
+ 0.00315797 0.00314607]</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2128,20 +2128,20 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145, 0.8066188197767145]</t>
+          <t>[0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373, 0.8241626794258373]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[np.float64(1108.875813223267), np.float64(1106.947333548097), np.float64(1110.804292898438), np.float64(1112.732772573609), np.float64(1105.018853872926), np.float64(1114.66125224878), np.float64(1116.589731923951), np.float64(1103.090374197755), np.float64(1118.518211599122), np.float64(1629.56532551941), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1627.63684584424), np.float64(1631.493805194581), np.float64(1133.946049000489), np.float64(1130.089089650148), np.float64(1633.422284869752), np.float64(1128.160609974977), np.float64(1122.375170949464), np.float64(1625.708366169069)]</t>
+          <t>[np.float64(1108.875813223267), np.float64(1110.804292898438), np.float64(1112.732772573609), np.float64(1106.947333548097), np.float64(1114.66125224878), np.float64(1116.589731923951), np.float64(1118.518211599122), np.float64(1105.018853872926), np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1128.160609974977), np.float64(1133.946049000489), np.float64(1629.56532551941), np.float64(1554.354618187745), np.float64(1122.375170949464), np.float64(1126.232130299806), np.float64(1552.426138512574), np.float64(1631.493805194581), np.float64(1124.303650624635)]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.00450479 0.00446557 0.0043951  0.00421767 0.00418477 0.00402431
- 0.00383346 0.00363806 0.00363647 0.0035054  0.00346471 0.00343567
- 0.00343073 0.00342909 0.00340377 0.00339141 0.00326345 0.00324484
- 0.00323998 0.00323751]</t>
+          <t>[0.00410832 0.00409009 0.00402154 0.00400928 0.00393111 0.00382833
+ 0.00372073 0.00372051 0.00369546 0.0036938  0.00361597 0.00359963
+ 0.00353567 0.00351928 0.00351489 0.00351242 0.00349077 0.00346449
+ 0.00346025 0.00345262]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2218,10 +2218,10 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[0.00422948 0.00421487 0.00417569 0.00414618 0.00403071 0.00400763
- 0.0038769  0.00381694 0.00374935 0.00370797 0.00367126 0.00364103
- 0.00355765 0.00344548 0.00341808 0.0033514  0.00333121 0.00332889
- 0.00332595 0.00332299]</t>
+          <t>[0.00425865 0.00424541 0.00420255 0.00417679 0.00406013 0.00403105
+ 0.00390422 0.00382953 0.00376285 0.00373252 0.00368972 0.00365169
+ 0.00357881 0.00345868 0.00343541 0.0033606  0.003319   0.00331665
+ 0.0033136  0.00331075]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2288,20 +2288,20 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705, 0.6678628389154705]</t>
+          <t>[0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692, 0.7507974481658692]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1128.160609974977), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1126.232130299806), np.float64(1122.375170949464), np.float64(1116.589731923951), np.float64(1133.946049000489), np.float64(1124.303650624635), np.float64(1114.66125224878), np.float64(1112.732772573609), np.float64(1110.804292898438), np.float64(1108.875813223267), np.float64(1135.87452867566), np.float64(1554.354618187745), np.float64(1556.283097862916), np.float64(1629.56532551941), np.float64(1631.493805194581), np.float64(1106.947333548097)]</t>
+          <t>[np.float64(1554.354618187745), np.float64(1132.017569325318), np.float64(1110.804292898438), np.float64(1130.089089650148), np.float64(1108.875813223267), np.float64(1112.732772573609), np.float64(1114.66125224878), np.float64(1556.283097862916), np.float64(1116.589731923951), np.float64(1552.426138512574), np.float64(1128.160609974977), np.float64(1118.518211599122), np.float64(1355.721211645143), np.float64(1353.792731969972), np.float64(1120.446691274293), np.float64(1357.649691320314), np.float64(1106.947333548097), np.float64(1351.864252294801), np.float64(1133.946049000489), np.float64(1550.497658837404)]</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[0.00411729 0.0040955  0.00403059 0.00394376 0.00394076 0.00392302
- 0.00390852 0.00390772 0.00389403 0.00387892 0.00386271 0.00380036
- 0.00370941 0.00358961 0.00351814 0.00351756 0.00346155 0.0034271
- 0.00341889 0.00337908]</t>
+          <t>[0.00345799 0.00338585 0.00338257 0.00338087 0.00337679 0.00337067
+ 0.00335541 0.00332998 0.00332863 0.00332458 0.00330432 0.00330257
+ 0.00328561 0.00328533 0.00327503 0.00326732 0.00326563 0.00326416
+ 0.00325996 0.00324601]</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2368,20 +2368,20 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445, 0.826555023923445]</t>
+          <t>[0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981, 0.8744019138755981]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[np.float64(1108.875813223267), np.float64(1110.804292898438), np.float64(1106.947333548097), np.float64(1112.732772573609), np.float64(1114.66125224878), np.float64(1116.589731923951), np.float64(1105.018853872926), np.float64(1425.146479951295), np.float64(1427.074959626466), np.float64(1118.518211599122), np.float64(1429.003439301637), np.float64(1423.218000276124), np.float64(1132.017569325318), np.float64(1130.089089650148), np.float64(1430.931918976808), np.float64(1554.354618187745), np.float64(1120.446691274293), np.float64(1484.929349881593), np.float64(1133.946049000489), np.float64(1556.283097862916)]</t>
+          <t>[np.float64(1108.875813223267), np.float64(1110.804292898438), np.float64(1106.947333548097), np.float64(1112.732772573609), np.float64(1114.66125224878), np.float64(1116.589731923951), np.float64(1105.018853872926), np.float64(1118.518211599122), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1130.089089650148), np.float64(1133.946049000489), np.float64(1128.160609974977), np.float64(1122.375170949464), np.float64(1427.074959626466), np.float64(1425.146479951295), np.float64(1554.354618187745), np.float64(1126.232130299806), np.float64(1429.003439301637), np.float64(1484.929349881593)]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.00385206 0.00382075 0.00373855 0.0037367  0.00363403 0.00349671
- 0.00340633 0.0033779  0.00337481 0.00333413 0.00331555 0.00329204
- 0.00324663 0.00321329 0.00320548 0.00318156 0.00317687 0.00315645
- 0.00314023 0.00313802]</t>
+          <t>[0.00416548 0.00413969 0.00404743 0.00404458 0.00391942 0.00377016
+ 0.00371162 0.0036018  0.00344341 0.00343468 0.00341277 0.00333683
+ 0.00330771 0.00327958 0.00324862 0.0032442  0.00322396 0.00320808
+ 0.00319532 0.0031889 ]</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2448,20 +2448,20 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>[0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708, 0.501427316644708]</t>
+          <t>[0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267, 0.5462231005709267]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[np.float64(1583.281813315309), np.float64(3043.14092741968), np.float64(1585.21029299048), np.float64(1581.353333640138), np.float64(2703.728504589601), np.float64(1579.424853964967), np.float64(1587.138772665651), np.float64(1577.496374289796), np.float64(954.5974392095954), np.float64(1589.067252340822), np.float64(1575.567894614625), np.float64(1060.663821343995), np.float64(1058.735341668824), np.float64(3045.069407094851), np.float64(952.6689595344246), np.float64(1062.592301019166), np.float64(1573.639414939454), np.float64(1099.233414847413), np.float64(1101.161894522584), np.float64(1064.520780694337)]</t>
+          <t>[np.float64(1583.281813315309), np.float64(3043.14092741968), np.float64(1581.353333640138), np.float64(1585.21029299048), np.float64(2703.728504589601), np.float64(1579.424853964967), np.float64(1587.138772665651), np.float64(1577.496374289796), np.float64(1575.567894614625), np.float64(954.5974392095954), np.float64(1589.067252340822), np.float64(1060.663821343995), np.float64(1058.735341668824), np.float64(3045.069407094851), np.float64(1573.639414939454), np.float64(1062.592301019166), np.float64(1099.233414847413), np.float64(952.6689595344246), np.float64(1101.161894522584), np.float64(1097.304935172242)]</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[0.0036716  0.00366777 0.00363866 0.00363526 0.00355478 0.00353977
- 0.0035343  0.00342331 0.00337624 0.00332439 0.00332187 0.00325569
- 0.00321406 0.00320621 0.00320534 0.00318109 0.00317256 0.00315133
- 0.00313905 0.00312521]</t>
+          <t>[0.00373287 0.00372543 0.0037027  0.00369128 0.00364021 0.00361067
+ 0.0035759  0.00349619 0.00339602 0.00339192 0.00335251 0.00330049
+ 0.00325784 0.00325398 0.0032457  0.00322434 0.00321766 0.00321351
+ 0.00320411 0.00317579]</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2528,20 +2528,20 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054, 0.5727931488801054]</t>
+          <t>[0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716, 0.6150636802810716]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[np.float64(1114.66125224878), np.float64(1116.589731923951), np.float64(1112.732772573609), np.float64(1118.518211599122), np.float64(1110.804292898438), np.float64(1120.446691274293), np.float64(1108.875813223267), np.float64(1066.449260369508), np.float64(1064.520780694337), np.float64(1062.592301019166), np.float64(1060.663821343995), np.float64(1068.377740044679), np.float64(1106.947333548097), np.float64(1058.735341668824), np.float64(1070.306219719849), np.float64(1083.805577446046), np.float64(1122.375170949464), np.float64(1085.734057121217), np.float64(1081.877097770875), np.float64(1105.018853872926)]</t>
+          <t>[np.float64(1060.663821343995), np.float64(1062.592301019166), np.float64(1058.735341668824), np.float64(1064.520780694337), np.float64(1066.449260369508), np.float64(1085.734057121217), np.float64(1087.662536796388), np.float64(1056.806861993653), np.float64(1068.377740044679), np.float64(1083.805577446046), np.float64(1101.161894522584), np.float64(1112.732772573609), np.float64(1099.233414847413), np.float64(1070.306219719849), np.float64(1089.591016471559), np.float64(1103.090374197755), np.float64(1105.018853872926), np.float64(1054.878382318482), np.float64(1106.947333548097), np.float64(1097.304935172242)]</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[0.00307374 0.003072   0.00304943 0.00304047 0.00300429 0.00297073
- 0.00295618 0.0029269  0.00292682 0.00292263 0.00291443 0.0029144
- 0.00291019 0.00289388 0.00288917 0.00288863 0.00288265 0.00288102
- 0.00286835 0.00286532]</t>
+          <t>[0.00360748 0.00357178 0.00356752 0.00354911 0.00351642 0.00348803
+ 0.00347772 0.00347469 0.00346818 0.00344707 0.00342893 0.00342618
+ 0.0034191  0.00341909 0.00341172 0.00340689 0.00339923 0.0033909
+ 0.00338961 0.00338367]</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2608,20 +2608,20 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317, 0.48012736056214317]</t>
+          <t>[0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568, 0.5198726394378568]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[np.float64(954.5974392095954), np.float64(3043.14092741968), np.float64(952.6689595344246), np.float64(1724.060829602785), np.float64(3045.069407094851), np.float64(1725.989309277955), np.float64(2674.801309462038), np.float64(950.7404798592538), np.float64(2996.857415215578), np.float64(2717.227862315798), np.float64(956.5259188847667), np.float64(2672.872829786867), np.float64(2998.785894890749), np.float64(3041.212447744509), np.float64(2703.728504589601), np.float64(1276.653544963136), np.float64(1002.809431088868), np.float64(1274.725065287965), np.float64(2730.727220041994), np.float64(1060.663821343995)]</t>
+          <t>[np.float64(3043.14092741968), np.float64(3045.069407094851), np.float64(1724.060829602785), np.float64(1725.989309277955), np.float64(2996.857415215578), np.float64(954.5974392095954), np.float64(2998.785894890749), np.float64(952.6689595344246), np.float64(2674.801309462038), np.float64(3041.212447744509), np.float64(1583.281813315309), np.float64(1581.353333640138), np.float64(1585.21029299048), np.float64(3008.428293266604), np.float64(1579.424853964967), np.float64(2717.227862315798), np.float64(1060.663821343995), np.float64(1587.138772665651), np.float64(1062.592301019166), np.float64(2994.928935540408)]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[0.00475212 0.00452998 0.00449913 0.00449804 0.00429438 0.00422508
- 0.00378825 0.0036901  0.00349825 0.00347877 0.0034501  0.00340275
- 0.00335259 0.00333961 0.00326865 0.00319589 0.00317923 0.0031201
- 0.00311561 0.00310913]</t>
+          <t>[0.00468387 0.00449755 0.004319   0.00407209 0.0038358  0.00382609
+ 0.00368802 0.00367449 0.00355986 0.00354534 0.00344836 0.00342205
+ 0.00338863 0.00335146 0.0033239  0.00330277 0.00329478 0.00325573
+ 0.0032325  0.00322435]</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2688,20 +2688,20 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>[0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358, 0.575318401405358]</t>
+          <t>[0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811, 0.5463328941589811]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[np.float64(3043.14092741968), np.float64(2703.728504589601), np.float64(2674.801309462038), np.float64(1583.281813315309), np.float64(3045.069407094851), np.float64(1585.21029299048), np.float64(1581.353333640138), np.float64(954.5974392095954), np.float64(1587.138772665651), np.float64(1579.424853964967), np.float64(2672.872829786867), np.float64(1577.496374289796), np.float64(952.6689595344246), np.float64(2701.800024914431), np.float64(1724.060829602785), np.float64(1589.067252340822), np.float64(1575.567894614625), np.float64(3041.212447744509), np.float64(1060.663821343995), np.float64(1573.639414939454)]</t>
+          <t>[np.float64(3043.14092741968), np.float64(1583.281813315309), np.float64(1585.21029299048), np.float64(1581.353333640138), np.float64(2703.728504589601), np.float64(3045.069407094851), np.float64(1587.138772665651), np.float64(954.5974392095954), np.float64(1579.424853964967), np.float64(952.6689595344246), np.float64(1577.496374289796), np.float64(1589.067252340822), np.float64(2674.801309462038), np.float64(1575.567894614625), np.float64(3041.212447744509), np.float64(1060.663821343995), np.float64(1573.639414939454), np.float64(1058.735341668824), np.float64(1099.233414847413), np.float64(1062.592301019166)]</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[0.00419548 0.00405872 0.00384257 0.00377047 0.00375447 0.00373404
- 0.00372895 0.00365842 0.00361902 0.00361782 0.0035052  0.00348298
- 0.00346666 0.00345496 0.00339797 0.00338788 0.00336805 0.00323859
- 0.00320398 0.00319714]</t>
+          <t>[0.00419517 0.00385675 0.00382822 0.00380647 0.00379211 0.0037265
+ 0.00372085 0.00371074 0.00368559 0.00354746 0.00354008 0.00349562
+ 0.00346042 0.00341282 0.00329904 0.00328424 0.00323064 0.00322228
+ 0.00322025 0.00321404]</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2773,15 +2773,15 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[np.float64(1729.846268628297), np.float64(964.23983758545), np.float64(1731.774748303468), np.float64(1727.917788953126), np.float64(962.3113579102792), np.float64(966.1683172606208), np.float64(1725.989309277955), np.float64(2996.857415215578), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(2998.785894890749), np.float64(954.5974392095954), np.float64(3043.14092741968), np.float64(956.5259188847667), np.float64(1733.703227978639), np.float64(3012.285252616945), np.float64(952.6689595344246), np.float64(960.3828782351084), np.float64(1724.060829602785), np.float64(3000.71437456592)]</t>
+          <t>[np.float64(1729.846268628297), np.float64(964.23983758545), np.float64(1731.774748303468), np.float64(1727.917788953126), np.float64(962.3113579102792), np.float64(966.1683172606208), np.float64(1725.989309277955), np.float64(2996.857415215578), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(2998.785894890749), np.float64(954.5974392095954), np.float64(3043.14092741968), np.float64(956.5259188847667), np.float64(3012.285252616945), np.float64(1733.703227978639), np.float64(952.6689595344246), np.float64(960.3828782351084), np.float64(1724.060829602785), np.float64(3000.71437456592)]</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[0.00667262 0.00601331 0.00595771 0.00587416 0.00572343 0.00569691
- 0.00544226 0.00539595 0.00531391 0.00528225 0.00526231 0.00525081
- 0.00505645 0.00497073 0.00496908 0.00496229 0.00488909 0.00480012
- 0.00476585 0.00475252]</t>
+          <t>[0.00665187 0.00600232 0.00591621 0.00588381 0.00571225 0.00569089
+ 0.00543434 0.00538476 0.00530617 0.00527819 0.00525428 0.00522784
+ 0.0049921  0.00496392 0.00496292 0.0049394  0.00485946 0.00479301
+ 0.00476697 0.00475302]</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2848,20 +2848,20 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475, 0.5497004357298475]</t>
+          <t>[0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913, 0.4581971677559913]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[np.float64(3004.571333916262), np.float64(3002.642854241091), np.float64(3006.499813591433), np.float64(3000.71437456592), np.float64(3016.142211967287), np.float64(2998.785894890749), np.float64(2994.928935540408), np.float64(2996.857415215578), np.float64(2993.000455865237), np.float64(3014.213732292117), np.float64(3008.428293266604), np.float64(3018.070691642458), np.float64(2991.071976190066), np.float64(3021.9276509928), np.float64(3010.356772941775), np.float64(3019.999171317629), np.float64(3012.285252616945), np.float64(2989.143496514895), np.float64(3035.427008718997), np.float64(3023.856130667971)]</t>
+          <t>[np.float64(2532.093813499392), np.float64(2510.880537072512), np.float64(2534.022293174562), np.float64(2512.809016747683), np.float64(2530.165333824221), np.float64(2522.451415123537), np.float64(2524.379894798708), np.float64(2503.166618371828), np.float64(2505.095098046999), np.float64(2508.952057397341), np.float64(2535.950772849733), np.float64(2501.238138696657), np.float64(2514.737496422853), np.float64(2507.02357772217), np.float64(2520.522935448366), np.float64(2526.308374473879), np.float64(2528.23685414905), np.float64(2537.879252524904), np.float64(2516.665976098025), np.float64(2518.594455773195)]</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.00346949 0.00341612 0.00331709 0.0033073  0.00325792 0.00323313
- 0.00322338 0.0032169  0.00316427 0.00311552 0.00307448 0.00306272
- 0.0030234  0.002978   0.0029373  0.00292766 0.002924   0.00284784
- 0.00284687 0.00283216]</t>
+          <t>[0.00321947 0.00316487 0.00316369 0.00316288 0.00314512 0.00311908
+ 0.00311456 0.00309033 0.003089   0.00308736 0.00308406 0.00307436
+ 0.00307125 0.00306466 0.00304534 0.00303804 0.00303018 0.00302947
+ 0.00300613 0.00299623]</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2928,20 +2928,20 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>[0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726, 0.4276960784313726]</t>
+          <t>[0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037, 0.4537037037037037]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(1729.846268628297), np.float64(3012.285252616945), np.float64(3010.356772941775), np.float64(2996.857415215578), np.float64(2998.785894890749), np.float64(964.23983758545), np.float64(954.5974392095954), np.float64(3000.71437456592), np.float64(3014.213732292117), np.float64(1727.917788953126), np.float64(962.3113579102792), np.float64(3008.428293266604), np.float64(3002.642854241091), np.float64(1731.774748303468), np.float64(956.5259188847667), np.float64(3031.570049368655), np.float64(3021.9276509928), np.float64(2994.928935540408)]</t>
+          <t>[np.float64(1729.846268628297), np.float64(1727.917788953126), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(1731.774748303468), np.float64(2996.857415215578), np.float64(2998.785894890749), np.float64(964.23983758545), np.float64(954.5974392095954), np.float64(3012.285252616945), np.float64(962.3113579102792), np.float64(956.5259188847667), np.float64(2696.014585888918), np.float64(966.1683172606208), np.float64(3000.71437456592), np.float64(3010.356772941775), np.float64(2994.928935540408), np.float64(3002.642854241091), np.float64(952.6689595344246), np.float64(1725.989309277955)]</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[0.00636177 0.00628754 0.00600789 0.00600765 0.00573197 0.00572035
- 0.00569811 0.00541455 0.00537276 0.00535895 0.00532712 0.0053127
- 0.00529585 0.00527148 0.00526003 0.00524852 0.00514969 0.00512461
- 0.00510584 0.00510189]</t>
+          <t>[0.00565134 0.00508469 0.00500739 0.00492808 0.00485498 0.00482454
+ 0.00475645 0.00466817 0.00464672 0.00464254 0.00449455 0.00448242
+ 0.00447769 0.00441341 0.0044109  0.00438617 0.00430783 0.00428586
+ 0.0042798  0.0042274 ]</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3008,20 +3008,20 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>[0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545, 0.5581427015250545]</t>
+          <t>[0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477, 0.5616830065359477]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[np.float64(1729.846268628297), np.float64(1731.774748303468), np.float64(964.23983758545), np.float64(3043.14092741968), np.float64(966.1683172606208), np.float64(1727.917788953126), np.float64(962.3113579102792), np.float64(1725.989309277955), np.float64(2996.857415215578), np.float64(2998.785894890749), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(1733.703227978639), np.float64(3045.069407094851), np.float64(3012.285252616945), np.float64(1724.060829602785), np.float64(3041.212447744509), np.float64(2994.928935540408), np.float64(3000.71437456592), np.float64(954.5974392095954)]</t>
+          <t>[np.float64(1729.846268628297), np.float64(964.23983758545), np.float64(962.3113579102792), np.float64(966.1683172606208), np.float64(1731.774748303468), np.float64(1727.917788953126), np.float64(2996.857415215578), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(2998.785894890749), np.float64(954.5974392095954), np.float64(1725.989309277955), np.float64(3043.14092741968), np.float64(956.5259188847667), np.float64(960.3828782351084), np.float64(3012.285252616945), np.float64(1733.703227978639), np.float64(952.6689595344246), np.float64(968.0967969357921), np.float64(3000.71437456592)]</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[0.00695132 0.00646114 0.00615588 0.00606871 0.00589891 0.00583457
- 0.00570502 0.00567351 0.0056565  0.0054745  0.00544276 0.0053812
- 0.00533835 0.00507535 0.00498959 0.00494114 0.00489165 0.00486103
- 0.00485417 0.00482208]</t>
+          <t>[0.00624646 0.00598093 0.00570402 0.00567881 0.0056688  0.00538744
+ 0.00520655 0.00519626 0.00512728 0.0050726  0.00503823 0.00495649
+ 0.00489728 0.00482068 0.00478716 0.00478457 0.00475581 0.00466256
+ 0.00458912 0.00458203]</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3088,20 +3088,20 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492, 0.3991582491582492]</t>
+          <t>[0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677, 0.3926767676767677]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[np.float64(962.3113579102792), np.float64(964.23983758545), np.float64(3023.856130667971), np.float64(3025.784610343142), np.float64(3012.285252616945), np.float64(3014.213732292117), np.float64(966.1683172606208), np.float64(960.3828782351084), np.float64(3010.356772941775), np.float64(3021.9276509928), np.float64(3027.713090018313), np.float64(3008.428293266604), np.float64(3033.498529043825), np.float64(3016.142211967287), np.float64(3006.499813591433), np.float64(3035.427008718997), np.float64(958.4543985599371), np.float64(956.5259188847667), np.float64(3004.571333916262), np.float64(2996.857415215578)]</t>
+          <t>[np.float64(962.3113579102792), np.float64(964.23983758545), np.float64(3023.856130667971), np.float64(3025.784610343142), np.float64(3012.285252616945), np.float64(966.1683172606208), np.float64(960.3828782351084), np.float64(3014.213732292117), np.float64(3010.356772941775), np.float64(3021.9276509928), np.float64(3027.713090018313), np.float64(3033.498529043825), np.float64(3008.428293266604), np.float64(3035.427008718997), np.float64(3016.142211967287), np.float64(958.4543985599371), np.float64(3006.499813591433), np.float64(956.5259188847667), np.float64(3004.571333916262), np.float64(968.0967969357921)]</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.00648044 0.00634532 0.00627941 0.00625416 0.00608318 0.00597944
- 0.00592061 0.00590796 0.0058745  0.00579502 0.00572668 0.00563694
- 0.00563246 0.00559247 0.00556507 0.00556147 0.00551787 0.00551592
- 0.00543263 0.00530005]</t>
+          <t>[0.00652945 0.00641028 0.00623295 0.0062095  0.00602846 0.00599889
+ 0.0059364  0.00592218 0.00581915 0.00574326 0.00568028 0.00561509
+ 0.00557989 0.00554802 0.00552733 0.00551494 0.00550643 0.00548648
+ 0.0053788  0.00531336]</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3168,20 +3168,20 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>[0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761, 0.4760942760942761]</t>
+          <t>[0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246, 0.46245791245791246]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[np.float64(3016.142211967287), np.float64(3014.213732292117), np.float64(3018.070691642458), np.float64(3006.499813591433), np.float64(3035.427008718997), np.float64(3012.285252616945), np.float64(958.4543985599371), np.float64(3008.428293266604), np.float64(3004.571333916262), np.float64(3010.356772941775), np.float64(956.5259188847667), np.float64(964.23983758545), np.float64(962.3113579102792), np.float64(3019.999171317629), np.float64(3002.642854241091), np.float64(3021.9276509928), np.float64(3033.498529043825), np.float64(3023.856130667971), np.float64(3000.71437456592), np.float64(3037.355488394167)]</t>
+          <t>[np.float64(3016.142211967287), np.float64(1727.917788953126), np.float64(3006.499813591433), np.float64(3004.571333916262), np.float64(3018.070691642458), np.float64(3014.213732292117), np.float64(3002.642854241091), np.float64(2993.000455865237), np.float64(2991.071976190066), np.float64(3000.71437456592), np.float64(3008.428293266604), np.float64(2964.073260737673), np.float64(2966.001740412844), np.float64(2981.429577814211), np.float64(2954.430862361819), np.float64(2956.359342036989), np.float64(2962.144781062502), np.float64(2989.143496514895), np.float64(2979.501098139041), np.float64(1729.846268628297)]</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[0.00592841 0.00553329 0.00543116 0.00516667 0.00508856 0.00508196
- 0.00504343 0.00495369 0.00495294 0.00489559 0.004848   0.00477574
- 0.00471229 0.00466835 0.00457037 0.00456024 0.00454256 0.00447577
- 0.00441788 0.00440279]</t>
+          <t>[0.0038002  0.00379754 0.00360961 0.0036063  0.00352619 0.00343479
+ 0.00341552 0.00333995 0.00330827 0.00329264 0.00327249 0.00325863
+ 0.00324724 0.00324452 0.00322913 0.00319053 0.00318391 0.00317606
+ 0.00317319 0.00317042]</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3248,20 +3248,20 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>[0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956, 0.33459595959595956]</t>
+          <t>[0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496, 0.36498316498316496]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[np.float64(964.23983758545), np.float64(962.3113579102792), np.float64(3025.784610343142), np.float64(3023.856130667971), np.float64(966.1683172606208), np.float64(968.0967969357921), np.float64(3012.285252616945), np.float64(3021.9276509928), np.float64(3027.713090018313), np.float64(960.3828782351084), np.float64(3010.356772941775), np.float64(3031.570049368655), np.float64(3014.213732292117), np.float64(3033.498529043825), np.float64(3029.641569693484), np.float64(3008.428293266604), np.float64(970.0252766109629), np.float64(3035.427008718997), np.float64(3037.355488394167), np.float64(3019.999171317629)]</t>
+          <t>[np.float64(956.5259188847667), np.float64(958.4543985599371), np.float64(962.3113579102792), np.float64(960.3828782351084), np.float64(964.23983758545), np.float64(954.5974392095954), np.float64(966.1683172606208), np.float64(3014.213732292117), np.float64(3012.285252616945), np.float64(3023.856130667971), np.float64(3010.356772941775), np.float64(3025.784610343142), np.float64(3006.499813591433), np.float64(3008.428293266604), np.float64(3016.142211967287), np.float64(3004.571333916262), np.float64(952.6689595344246), np.float64(3021.9276509928), np.float64(2994.928935540408), np.float64(2996.857415215578)]</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[0.00672326 0.00669569 0.00669557 0.00667615 0.0065646  0.00601226
- 0.00593691 0.00591082 0.00589508 0.0057979  0.00571341 0.00558295
- 0.00557692 0.00555992 0.00534419 0.00526798 0.00524022 0.00516965
- 0.00508257 0.00493308]</t>
+          <t>[0.00666363 0.00655161 0.00651323 0.00639312 0.00606672 0.00569239
+ 0.00542665 0.00521761 0.0052126  0.00519983 0.00505366 0.00503175
+ 0.00503139 0.00496564 0.00495792 0.00492846 0.00492316 0.00483316
+ 0.00481036 0.00478776]</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -3328,20 +3328,20 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174, 0.39175084175084174]</t>
+          <t>[0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084, 0.4334175084175084]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[np.float64(962.3113579102792), np.float64(964.23983758545), np.float64(3023.856130667971), np.float64(3025.784610343142), np.float64(966.1683172606208), np.float64(3012.285252616945), np.float64(960.3828782351084), np.float64(3014.213732292117), np.float64(3010.356772941775), np.float64(3021.9276509928), np.float64(3027.713090018313), np.float64(3033.498529043825), np.float64(3008.428293266604), np.float64(3035.427008718997), np.float64(3031.570049368655), np.float64(3006.499813591433), np.float64(3016.142211967287), np.float64(958.4543985599371), np.float64(968.0967969357921), np.float64(3029.641569693484)]</t>
+          <t>[np.float64(962.3113579102792), np.float64(964.23983758545), np.float64(3023.856130667971), np.float64(3025.784610343142), np.float64(3012.285252616945), np.float64(966.1683172606208), np.float64(3014.213732292117), np.float64(960.3828782351084), np.float64(3010.356772941775), np.float64(3021.9276509928), np.float64(3027.713090018313), np.float64(3033.498529043825), np.float64(3008.428293266604), np.float64(3035.427008718997), np.float64(3016.142211967287), np.float64(3006.499813591433), np.float64(958.4543985599371), np.float64(3031.570049368655), np.float64(956.5259188847667), np.float64(3004.571333916262)]</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.00637398 0.00624591 0.00609429 0.00607928 0.00582643 0.00581809
- 0.00576821 0.00563656 0.00562234 0.00560256 0.00556895 0.00545221
- 0.00535344 0.00528487 0.00528426 0.00523976 0.00519955 0.00519546
- 0.00516445 0.00514918]</t>
+          <t>[0.00673999 0.00661333 0.00654527 0.00651911 0.00629399 0.00617216
+ 0.00615086 0.00612141 0.00608034 0.00603462 0.00597537 0.00587267
+ 0.00580971 0.00574747 0.0057266  0.00569652 0.00562693 0.00560799
+ 0.00556032 0.00553681]</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -3413,15 +3413,15 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1130.089089650148), np.float64(1120.446691274293), np.float64(1132.017569325318), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1135.87452867566), np.float64(1116.589731923951), np.float64(1137.803008350831), np.float64(1114.66125224878), np.float64(1041.379024592286), np.float64(1043.307504267457), np.float64(1039.450544917115), np.float64(1139.731488026002), np.float64(1509.999585658815), np.float64(1511.928065333986), np.float64(1037.522065241944)]</t>
+          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1130.089089650148), np.float64(1120.446691274293), np.float64(1132.017569325318), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1135.87452867566), np.float64(1116.589731923951), np.float64(1137.803008350831), np.float64(1114.66125224878), np.float64(1041.379024592286), np.float64(1043.307504267457), np.float64(1039.450544917115), np.float64(1139.731488026002), np.float64(1037.522065241944), np.float64(1045.235983942628), np.float64(1112.732772573609)]</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[0.0041459  0.00412626 0.00410805 0.00405986 0.00404553 0.00396849
- 0.00394846 0.00381483 0.00379161 0.00362748 0.00355942 0.0033989
- 0.00328215 0.00316856 0.00314492 0.0031183  0.00309249 0.00307053
- 0.00306272 0.00302584]</t>
+          <t>[0.00438742 0.00436463 0.00434631 0.00428785 0.00427299 0.00417871
+ 0.00415656 0.00399671 0.00397871 0.00377987 0.00372176 0.0035252
+ 0.00342162 0.00332759 0.0032901  0.00328588 0.00319933 0.00319765
+ 0.00315116 0.00307112]</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3493,15 +3493,15 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[np.float64(1128.160609974977), np.float64(1126.232130299806), np.float64(1130.089089650148), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1116.589731923951), np.float64(1135.87452867566), np.float64(1114.66125224878), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1137.803008350831), np.float64(1560.140057213258), np.float64(1558.211577538087), np.float64(1500.35718728296), np.float64(1504.214146633302), np.float64(1509.999585658815)]</t>
+          <t>[np.float64(1128.160609974977), np.float64(1126.232130299806), np.float64(1130.089089650148), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1132.017569325318), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1133.946049000489), np.float64(1116.589731923951), np.float64(1135.87452867566), np.float64(1114.66125224878), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1112.732772573609), np.float64(1137.803008350831), np.float64(1390.433845798219), np.float64(1392.36232547339), np.float64(1558.211577538087), np.float64(1405.861683199586)]</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[0.00365842 0.00364569 0.00358944 0.00356996 0.00349984 0.00346218
- 0.00340626 0.00325018 0.00324219 0.00304497 0.00296343 0.00281276
- 0.00276035 0.00272038 0.00265559 0.00263104 0.00263008 0.00262613
- 0.00259184 0.00258394]</t>
+          <t>[0.00379743 0.00378002 0.00373122 0.00370519 0.00364228 0.00359581
+ 0.00356128 0.00341307 0.00336373 0.00323273 0.00304799 0.00302007
+ 0.00284224 0.00284068 0.00276273 0.0027089  0.00268874 0.0026862
+ 0.00266937 0.00265822]</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3568,20 +3568,20 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853, 0.7351851851851853]</t>
+          <t>[0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889, 0.7388888888888889]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[np.float64(1128.160609974977), np.float64(1130.089089650148), np.float64(1126.232130299806), np.float64(1132.017569325318), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1133.946049000489), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1135.87452867566), np.float64(1116.589731923951), np.float64(1509.999585658815), np.float64(1511.928065333986), np.float64(1137.803008350831), np.float64(1515.785024684327), np.float64(1513.856545009157), np.float64(1517.713504359498), np.float64(1519.641984034669), np.float64(1041.379024592286), np.float64(1508.071105983644)]</t>
+          <t>[np.float64(1128.160609974977), np.float64(1130.089089650148), np.float64(1126.232130299806), np.float64(1132.017569325318), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1133.946049000489), np.float64(1560.140057213258), np.float64(1558.211577538087), np.float64(1511.928065333986), np.float64(1509.999585658815), np.float64(1513.856545009157), np.float64(1515.785024684327), np.float64(1556.283097862916), np.float64(1517.713504359498), np.float64(1120.446691274293), np.float64(1519.641984034669), np.float64(1508.071105983644), np.float64(1521.57046370984), np.float64(1135.87452867566)]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.00370651 0.00369313 0.00368402 0.00365039 0.00363627 0.00358107
- 0.00355689 0.00351155 0.00339493 0.00338498 0.00322971 0.00314932
- 0.00314913 0.0031295  0.00311989 0.00311963 0.00308208 0.00306789
- 0.00306451 0.00306327]</t>
+          <t>[0.00373308 0.00371459 0.00370964 0.00365926 0.00365083 0.00355908
+ 0.00355555 0.00354468 0.00354283 0.00350879 0.00349749 0.00349587
+ 0.00348638 0.00347489 0.00345789 0.00344146 0.00343723 0.00343379
+ 0.00340028 0.00337209]</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3653,15 +3653,15 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[np.float64(1128.160609974977), np.float64(1126.232130299806), np.float64(1130.089089650148), np.float64(1124.303650624635), np.float64(1041.379024592286), np.float64(1039.450544917115), np.float64(1043.307504267457), np.float64(1132.017569325318), np.float64(1122.375170949464), np.float64(1037.522065241944), np.float64(1133.946049000489), np.float64(1045.235983942628), np.float64(1035.593585566773), np.float64(1120.446691274293), np.float64(1033.665105891602), np.float64(1135.87452867566), np.float64(1047.164463617799), np.float64(1031.736626216432), np.float64(1118.518211599122), np.float64(1029.808146541261)]</t>
+          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1130.089089650148), np.float64(1122.375170949464), np.float64(1132.017569325318), np.float64(1041.379024592286), np.float64(1039.450544917115), np.float64(1043.307504267457), np.float64(1133.946049000489), np.float64(1120.446691274293), np.float64(1037.522065241944), np.float64(1045.235983942628), np.float64(1035.593585566773), np.float64(1135.87452867566), np.float64(1118.518211599122), np.float64(1033.665105891602), np.float64(1047.164463617799), np.float64(1031.736626216432), np.float64(1137.803008350831)]</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[0.0046211  0.00462082 0.00458433 0.00457817 0.00455729 0.00451974
- 0.004501   0.00449457 0.00444593 0.00442985 0.00433997 0.00433111
- 0.00429804 0.0042358  0.00414485 0.00409583 0.00407666 0.00400443
- 0.00397186 0.00382435]</t>
+          <t>[0.00469412 0.00468408 0.00465862 0.00463303 0.00454983 0.0045397
+ 0.00445543 0.00442347 0.00439523 0.00439042 0.00436721 0.00433808
+ 0.00422418 0.00420666 0.00416099 0.00412026 0.0040439  0.00397132
+ 0.00387935 0.00386524]</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3733,15 +3733,15 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[np.float64(1130.089089650148), np.float64(1128.160609974977), np.float64(1132.017569325318), np.float64(1126.232130299806), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1133.946049000489), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1116.589731923951), np.float64(1114.66125224878), np.float64(1388.505366123048), np.float64(1135.87452867566), np.float64(1112.732772573609), np.float64(1390.433845798219), np.float64(1110.804292898438), np.float64(1039.450544917115), np.float64(1041.379024592286), np.float64(1037.522065241944), np.float64(1137.803008350831)]</t>
+          <t>[np.float64(1130.089089650148), np.float64(1128.160609974977), np.float64(1126.232130299806), np.float64(1132.017569325318), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1133.946049000489), np.float64(1388.505366123048), np.float64(1116.589731923951), np.float64(1114.66125224878), np.float64(1390.433845798219), np.float64(1135.87452867566), np.float64(1112.732772573609), np.float64(1386.576886447877), np.float64(1110.804292898438), np.float64(1392.36232547339), np.float64(1039.450544917115), np.float64(1041.379024592286)]</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[0.00441473 0.00438461 0.00436795 0.00432658 0.00427727 0.0042348
- 0.00422149 0.00421762 0.00420685 0.00414729 0.0040512  0.00397106
- 0.00393039 0.00392058 0.00381016 0.00372115 0.00356136 0.00353299
- 0.00351467 0.00349257]</t>
+          <t>[0.00433057 0.00432248 0.00427185 0.00425847 0.0042162  0.00416999
+ 0.00414235 0.00410564 0.00408433 0.00407528 0.00402324 0.00390586
+ 0.00388055 0.0037737  0.0037501  0.0036154  0.00353844 0.00352242
+ 0.00349965 0.00347155]</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3888,20 +3888,20 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>[0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091, 0.7826108110738091]</t>
+          <t>[0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975, 0.7354644090886975]</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[np.float64(1128.160609974977), np.float64(1130.089089650148), np.float64(1126.232130299806), np.float64(1124.303650624635), np.float64(1132.017569325318), np.float64(1122.375170949464), np.float64(1120.446691274293), np.float64(1118.518211599122), np.float64(1133.946049000489), np.float64(1116.589731923951), np.float64(1114.66125224878), np.float64(1135.87452867566), np.float64(1388.505366123048), np.float64(1112.732772573609), np.float64(1390.433845798219), np.float64(1039.450544917115), np.float64(1386.576886447877), np.float64(1041.379024592286), np.float64(1037.522065241944), np.float64(1043.307504267457)]</t>
+          <t>[np.float64(1126.232130299806), np.float64(1128.160609974977), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1130.089089650148), np.float64(1120.446691274293), np.float64(1558.211577538087), np.float64(1556.283097862916), np.float64(1132.017569325318), np.float64(1560.140057213258), np.float64(1118.518211599122), np.float64(1554.354618187745), np.float64(1646.921642595948), np.float64(1562.068536888429), np.float64(1133.946049000489), np.float64(1575.567894614625), np.float64(1573.639414939454), np.float64(1571.710935264284), np.float64(1577.496374289796), np.float64(1116.589731923951)]</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[0.00420753 0.0041886  0.00416374 0.00409215 0.00408996 0.00403209
- 0.00397896 0.00388926 0.00388905 0.00375281 0.00357822 0.00356612
- 0.00355541 0.00335393 0.0033229  0.00325285 0.00324365 0.00323414
- 0.0032108  0.00314264]</t>
+          <t>[0.00440567 0.00437716 0.0043109  0.00422196 0.00418367 0.0040895
+ 0.00399578 0.00396913 0.00391997 0.00389798 0.00383249 0.00370239
+ 0.00368065 0.00365548 0.00360586 0.00354036 0.00353227 0.00352324
+ 0.00350315 0.0034981 ]</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3968,20 +3968,20 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>[0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169, 0.8521870286576169]</t>
+          <t>[0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975, 0.8974358974358975]</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1128.160609974977), np.float64(1133.946049000489), np.float64(1126.232130299806), np.float64(1116.589731923951), np.float64(1118.518211599122), np.float64(1114.66125224878), np.float64(1124.303650624635), np.float64(1120.446691274293), np.float64(1122.375170949464), np.float64(1112.732772573609), np.float64(1110.804292898438), np.float64(1388.505366123048), np.float64(1135.87452867566), np.float64(1390.433845798219), np.float64(1108.875813223267), np.float64(1039.450544917115), np.float64(1037.522065241944), np.float64(1041.379024592286)]</t>
+          <t>[np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1128.160609974977), np.float64(1116.589731923951), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1114.66125224878), np.float64(1126.232130299806), np.float64(1388.505366123048), np.float64(1120.446691274293), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1112.732772573609), np.float64(1110.804292898438), np.float64(1135.87452867566), np.float64(1390.433845798219), np.float64(1039.450544917115), np.float64(1037.522065241944), np.float64(1041.379024592286), np.float64(1035.593585566773)]</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[0.0044926  0.00448156 0.00442831 0.00437368 0.00435504 0.00434743
- 0.0043407  0.00432028 0.00431354 0.00428979 0.00428033 0.00427088
- 0.00412868 0.00411551 0.00410585 0.00392177 0.00391618 0.00382902
- 0.0038064  0.00376976]</t>
+          <t>[0.00431741 0.00431203 0.00426514 0.00423262 0.00422833 0.00422259
+ 0.00420566 0.00420396 0.00419177 0.00417089 0.00416982 0.00415052
+ 0.00414971 0.00400817 0.00400192 0.00394056 0.00390945 0.0038907
+ 0.00385197 0.00381662]</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>[0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936, 0.8413848631239936]</t>
+          <t>[0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512, 0.859903381642512]</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -4058,10 +4058,10 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[0.00466908 0.00465067 0.00457134 0.00448968 0.00446525 0.00441093
- 0.00440821 0.00439794 0.00438017 0.00435469 0.00434617 0.00433107
- 0.00421064 0.00416811 0.00403179 0.00381842 0.00369012 0.00353961
- 0.00333074 0.00329645]</t>
+          <t>[0.00461441 0.00459802 0.004519   0.00444277 0.00441466 0.00436974
+ 0.00436385 0.00434782 0.00434251 0.00430994 0.0042991  0.00429597
+ 0.00418104 0.00412956 0.0040098  0.00380499 0.00366313 0.00353743
+ 0.00329164 0.00325541]</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -4133,15 +4133,15 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>[np.float64(1128.160609974977), np.float64(1130.089089650148), np.float64(1126.232130299806), np.float64(1132.017569325318), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1120.446691274293), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1116.589731923951), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1114.66125224878), np.float64(1135.87452867566), np.float64(1390.433845798219), np.float64(1392.36232547339), np.float64(1558.211577538087), np.float64(1112.732772573609), np.float64(973.8822359613046), np.float64(971.9537562861337)]</t>
+          <t>[np.float64(1128.160609974977), np.float64(1130.089089650148), np.float64(1126.232130299806), np.float64(1132.017569325318), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1120.446691274293), np.float64(1133.946049000489), np.float64(1118.518211599122), np.float64(1116.589731923951), np.float64(1114.66125224878), np.float64(1135.87452867566), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1390.433845798219), np.float64(1392.36232547339), np.float64(1112.732772573609), np.float64(1558.211577538087), np.float64(973.8822359613046), np.float64(971.9537562861337)]</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[0.00388838 0.00388558 0.00382737 0.00378745 0.00374233 0.00367062
- 0.00360646 0.0035697  0.00351637 0.00339812 0.00328572 0.00327091
- 0.00325417 0.0032253  0.00320583 0.0031497  0.0031318  0.0030744
- 0.00305229 0.00303619]</t>
+          <t>[0.00393256 0.00392719 0.00387392 0.00382844 0.0037909  0.0037228
+ 0.00366137 0.00361146 0.00357197 0.00345493 0.00331213 0.00326858
+ 0.00324572 0.00324054 0.00323244 0.00316844 0.00313382 0.0030838
+ 0.00306493 0.00305084]</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -4208,20 +4208,20 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>[0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881, 0.7565619967793881]</t>
+          <t>[0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492, 0.6884057971014492]</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[np.float64(1130.089089650148), np.float64(1132.017569325318), np.float64(1128.160609974977), np.float64(1114.66125224878), np.float64(1112.732772573609), np.float64(1116.589731923951), np.float64(1110.804292898438), np.float64(1118.518211599122), np.float64(1126.232130299806), np.float64(1120.446691274293), np.float64(1108.875813223267), np.float64(1124.303650624635), np.float64(1133.946049000489), np.float64(1122.375170949464), np.float64(1106.947333548097), np.float64(1105.018853872926), np.float64(1135.87452867566), np.float64(1103.090374197755), np.float64(1137.803008350831), np.float64(1392.36232547339)]</t>
+          <t>[np.float64(1130.089089650148), np.float64(1128.160609974977), np.float64(1132.017569325318), np.float64(1126.232130299806), np.float64(1124.303650624635), np.float64(1133.946049000489), np.float64(1122.375170949464), np.float64(1392.36232547339), np.float64(1120.446691274293), np.float64(1390.433845798219), np.float64(1118.518211599122), np.float64(1394.290805148561), np.float64(1116.589731923951), np.float64(1396.219284823732), np.float64(1114.66125224878), np.float64(1398.147764498902), np.float64(1112.732772573609), np.float64(1554.354618187745), np.float64(1550.497658837404), np.float64(1548.569179162233)]</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[0.00400638 0.00397918 0.00395239 0.00391959 0.00391045 0.00390958
- 0.00388456 0.00388317 0.00388052 0.00384363 0.00383921 0.0038286
- 0.00382808 0.00381577 0.00374717 0.00357208 0.00353984 0.00328709
- 0.00315469 0.00309409]</t>
+          <t>[0.00341467 0.00336469 0.00333072 0.0032656  0.00316442 0.00308114
+ 0.00307714 0.00305733 0.00302847 0.00301084 0.00299961 0.00299601
+ 0.00296523 0.00293139 0.00292979 0.00287272 0.0028712  0.00286864
+ 0.00285519 0.00284445]</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -4288,20 +4288,20 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>[0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052, 0.8268921095008052]</t>
+          <t>[0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353, 0.8309178743961353]</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[np.float64(1110.804292898438), np.float64(1112.732772573609), np.float64(1108.875813223267), np.float64(1114.66125224878), np.float64(1132.017569325318), np.float64(1116.589731923951), np.float64(1133.946049000489), np.float64(1106.947333548097), np.float64(1130.089089650148), np.float64(1135.87452867566), np.float64(1118.518211599122), np.float64(929.5272034323739), np.float64(1128.160609974977), np.float64(1105.018853872926), np.float64(1120.446691274293), np.float64(1126.232130299806), np.float64(1124.303650624635), np.float64(1122.375170949464), np.float64(1137.803008350831), np.float64(964.23983758545)]</t>
+          <t>[np.float64(1132.017569325318), np.float64(1130.089089650148), np.float64(1133.946049000489), np.float64(1128.160609974977), np.float64(1116.589731923951), np.float64(1114.66125224878), np.float64(1112.732772573609), np.float64(1118.518211599122), np.float64(1126.232130299806), np.float64(1124.303650624635), np.float64(1135.87452867566), np.float64(1110.804292898438), np.float64(1120.446691274293), np.float64(1122.375170949464), np.float64(1108.875813223267), np.float64(1137.803008350831), np.float64(1106.947333548097), np.float64(929.5272034323739), np.float64(1139.731488026002), np.float64(1105.018853872926)]</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[0.00515719 0.00515301 0.00500557 0.0049879  0.00482724 0.00482302
- 0.00481168 0.00475444 0.00469361 0.00461253 0.0046066  0.00442923
- 0.00442594 0.00431256 0.00430619 0.00423964 0.00419214 0.00417126
- 0.00416385 0.0041148 ]</t>
+          <t>[0.00547545 0.00544444 0.00534968 0.00526411 0.0051821  0.00517578
+ 0.00517235 0.00513706 0.00511625 0.00505298 0.00504032 0.005034
+ 0.00499909 0.00497646 0.00477573 0.00450473 0.00445582 0.00407617
+ 0.00399874 0.00399633]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -4368,20 +4368,20 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>[0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425, 0.46428571428571425]</t>
+          <t>[0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237, 0.5238095238095237]</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(950.7404798592538), np.float64(946.8835205089117), np.float64(944.9550408337414), np.float64(937.2411221330576), np.float64(943.0265611585701), np.float64(935.3126424578863), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(952.6689595344246), np.float64(1047.164463617799), np.float64(1049.092943292969), np.float64(1554.354618187745), np.float64(1556.283097862916), np.float64(1558.211577538087), np.float64(1560.140057213258), np.float64(1045.235983942628)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(933.3841627827155), np.float64(948.812000184083), np.float64(950.7404798592538), np.float64(946.8835205089117), np.float64(944.9550408337414), np.float64(935.3126424578863), np.float64(937.2411221330576), np.float64(943.0265611585701), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(952.6689595344246), np.float64(1047.164463617799), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1049.092943292969), np.float64(1558.211577538087), np.float64(1560.140057213258), np.float64(1045.235983942628)]</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[0.00507397 0.00472795 0.00438437 0.0043792  0.0043562  0.00433949
- 0.00428338 0.00425064 0.00424674 0.00424606 0.00421846 0.00421509
- 0.00418447 0.0040454  0.003963   0.00396241 0.00395747 0.00392066
- 0.00391417 0.00390006]</t>
+          <t>[0.0051658  0.00484731 0.0045175  0.00451151 0.00448097 0.00446338
+ 0.00440228 0.00438637 0.0043829  0.00436284 0.00434294 0.00433325
+ 0.00429917 0.0040874  0.00401349 0.00400651 0.00400473 0.00398558
+ 0.00398182 0.00395216]</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -4453,15 +4453,15 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>[np.float64(1509.999585658815), np.float64(1508.071105983644), np.float64(1511.928065333986), np.float64(1506.142626308473), np.float64(1602.566610067018), np.float64(1513.856545009157), np.float64(1515.785024684327), np.float64(1604.495089742189), np.float64(1504.214146633302), np.float64(1500.35718728296), np.float64(1502.285666958131), np.float64(1498.428707607789), np.float64(1517.713504359498), np.float64(1496.500227932618), np.float64(1600.638130391847), np.float64(1494.571748257448), np.float64(1519.641984034669), np.float64(1521.57046370984), np.float64(1606.42356941736), np.float64(1492.643268582277)]</t>
+          <t>[np.float64(1602.566610067018), np.float64(1600.638130391847), np.float64(1604.495089742189), np.float64(1598.709650716676), np.float64(1606.42356941736), np.float64(1596.781171041505), np.float64(1594.852691366334), np.float64(1592.924211691163), np.float64(1608.35204909253), np.float64(1515.785024684327), np.float64(1517.713504359498), np.float64(1513.856545009157), np.float64(1511.928065333986), np.float64(1509.999585658815), np.float64(1519.641984034669), np.float64(1508.071105983644), np.float64(1282.438983988648), np.float64(1521.57046370984), np.float64(1590.995732015992), np.float64(1280.510504313478)]</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[0.00516091 0.00513841 0.00512997 0.00510057 0.00508246 0.00508229
- 0.00505219 0.0050377  0.00502469 0.00499592 0.00498161 0.00497608
- 0.00496219 0.00494284 0.00492051 0.0048755  0.00484676 0.0047679
- 0.00473764 0.00473528]</t>
+          <t>[0.00656639 0.00649968 0.00635379 0.00623776 0.00583253 0.00581186
+ 0.00528585 0.00488135 0.00484787 0.00484055 0.00476461 0.00474312
+ 0.00471522 0.00466086 0.00459053 0.00451857 0.00451184 0.00450173
+ 0.00447923 0.0044652 ]</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -4528,20 +4528,20 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>[0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506, 0.36507936507936506]</t>
+          <t>[0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953, 0.3452380952380953]</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>[np.float64(1560.140057213258), np.float64(1562.068536888429), np.float64(1558.211577538087), np.float64(1563.9970165636), np.float64(1565.925496238771), np.float64(1556.283097862916), np.float64(1554.354618187745), np.float64(1567.853975913942), np.float64(1552.426138512574), np.float64(1569.782455589112), np.float64(1571.710935264284), np.float64(1550.497658837404), np.float64(1573.639414939454), np.float64(1392.36232547339), np.float64(1394.290805148561), np.float64(1575.567894614625), np.float64(1396.219284823732), np.float64(1577.496374289796), np.float64(1390.433845798219), np.float64(1398.147764498902)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(950.7404798592538), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(952.6689595344246), np.float64(935.3126424578863), np.float64(946.8835205089117), np.float64(937.2411221330576), np.float64(944.9550408337414), np.float64(954.5974392095954), np.float64(939.1696018082284), np.float64(943.0265611585701), np.float64(941.0980814833993), np.float64(956.5259188847667), np.float64(1558.211577538087), np.float64(1556.283097862916), np.float64(1392.36232547339), np.float64(1394.290805148561), np.float64(1560.140057213258)]</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>[0.00484916 0.0048148  0.00480344 0.00478105 0.00477544 0.0047697
- 0.00472119 0.00466515 0.00461013 0.00460588 0.0046025  0.00450976
- 0.00450352 0.00448601 0.00448375 0.00446051 0.00444373 0.00444301
- 0.00443805 0.00437954]</t>
+          <t>[0.00455373 0.00448321 0.00439386 0.00432009 0.00431499 0.00428076
+ 0.00416849 0.0041648  0.00406018 0.00402438 0.00397261 0.00396735
+ 0.00393913 0.00391929 0.00353701 0.00352598 0.00351207 0.00350178
+ 0.00349788 0.00349543]</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -4608,20 +4608,20 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>[0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413, 0.48412698412698413]</t>
+          <t>[0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015, 0.5515873015873015]</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(946.8835205089117), np.float64(948.812000184083), np.float64(944.9550408337414), np.float64(943.0265611585701), np.float64(950.7404798592538), np.float64(941.0980814833993), np.float64(933.3841627827155), np.float64(939.1696018082284), np.float64(952.6689595344246), np.float64(937.2411221330576), np.float64(935.3126424578863), np.float64(1049.092943292969), np.float64(1047.164463617799), np.float64(954.5974392095954), np.float64(1554.354618187745), np.float64(1045.235983942628), np.float64(1051.021422968141), np.float64(1556.283097862916)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(950.7404798592538), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(952.6689595344246), np.float64(935.3126424578863), np.float64(944.9550408337414), np.float64(937.2411221330576), np.float64(943.0265611585701), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(1047.164463617799), np.float64(1045.235983942628), np.float64(954.5974392095954), np.float64(1049.092943292969), np.float64(1043.307504267457), np.float64(1556.283097862916), np.float64(1560.140057213258)]</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>[0.00599313 0.0052821  0.00481151 0.0048081  0.00479552 0.00477802
- 0.00476103 0.00470878 0.00467225 0.00464961 0.00462499 0.00461903
- 0.00451178 0.00442341 0.0044081  0.004319   0.00412021 0.0041166
- 0.00405798 0.00405511]</t>
+          <t>[0.00555425 0.00521999 0.00489207 0.00487533 0.00486716 0.00478039
+ 0.00473745 0.00470827 0.00468434 0.00468043 0.00462542 0.00462123
+ 0.00459658 0.00449308 0.00439768 0.0043745  0.00435595 0.00419545
+ 0.00416801 0.00415371]</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -4688,20 +4688,20 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>[0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656, 0.42240418894830656]</t>
+          <t>[0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764, 0.31433823529411764]</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(935.3126424578863), np.float64(956.5259188847667), np.float64(937.2411221330576), np.float64(944.9550408337414), np.float64(939.1696018082284), np.float64(943.0265611585701), np.float64(941.0980814833993), np.float64(1394.290805148561), np.float64(1392.36232547339), np.float64(1396.219284823732), np.float64(1390.433845798219), np.float64(1398.147764498902)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(935.3126424578863), np.float64(956.5259188847667), np.float64(937.2411221330576), np.float64(944.9550408337414), np.float64(939.1696018082284), np.float64(1394.290805148561), np.float64(943.0265611585701), np.float64(941.0980814833993), np.float64(1396.219284823732), np.float64(1392.36232547339), np.float64(1398.147764498902), np.float64(1390.433845798219)]</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[0.00566898 0.00515674 0.00504175 0.00496383 0.00485048 0.00473651
- 0.00469304 0.00451082 0.00445562 0.00439819 0.00435646 0.00434672
- 0.00427238 0.00426329 0.00423976 0.00412384 0.00408064 0.00407886
- 0.00397679 0.00395969]</t>
+          <t>[0.0054557  0.00498312 0.00487513 0.00479778 0.00469527 0.00456425
+ 0.00454262 0.00432793 0.00430111 0.0042775  0.00418866 0.00415479
+ 0.0040961  0.00407544 0.00406598 0.00405017 0.00403809 0.00401852
+ 0.00391912 0.00389384]</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -4773,15 +4773,15 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[np.float64(1600.638130391847), np.float64(1598.709650716676), np.float64(1602.566610067018), np.float64(3050.854846120364), np.float64(1596.781171041505), np.float64(1604.495089742189), np.float64(1606.42356941736), np.float64(1594.852691366334), np.float64(1592.924211691163), np.float64(929.5272034323739), np.float64(1492.643268582277), np.float64(1608.35204909253), np.float64(1494.571748257448), np.float64(1490.714788907106), np.float64(1496.500227932618), np.float64(1488.786309231935), np.float64(1704.776032851076), np.float64(1498.428707607789), np.float64(1590.995732015992), np.float64(1486.857829556764)]</t>
+          <t>[np.float64(1598.709650716676), np.float64(1600.638130391847), np.float64(1602.566610067018), np.float64(1596.781171041505), np.float64(1492.643268582277), np.float64(1494.571748257448), np.float64(3050.854846120364), np.float64(1496.500227932618), np.float64(1490.714788907106), np.float64(1498.428707607789), np.float64(1604.495089742189), np.float64(1488.786309231935), np.float64(1500.35718728296), np.float64(1594.852691366334), np.float64(1502.285666958131), np.float64(1486.857829556764), np.float64(1606.42356941736), np.float64(929.5272034323739), np.float64(1504.214146633302), np.float64(1484.929349881593)]</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>[0.00588097 0.00578444 0.00567688 0.00533921 0.00530672 0.00523483
- 0.00458977 0.00452266 0.00385215 0.00360808 0.00344234 0.00338649
- 0.00338456 0.00338196 0.00332041 0.00326855 0.00325305 0.00318552
- 0.00312986 0.00309397]</t>
+          <t>[0.00593456 0.00593376 0.00558921 0.0054745  0.00530911 0.00528281
+ 0.00525339 0.00522598 0.00516589 0.00506898 0.00500425 0.00491943
+ 0.00479424 0.00462823 0.00462045 0.00455448 0.00424037 0.00421855
+ 0.00420579 0.00399085]</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -4928,20 +4928,20 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>[0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082, 0.464349376114082]</t>
+          <t>[0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813, 0.38290998217468813]</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(944.9550408337414), np.float64(935.3126424578863), np.float64(943.0265611585701), np.float64(937.2411221330576), np.float64(941.0980814833993), np.float64(939.1696018082284), np.float64(956.5259188847667), np.float64(1392.36232547339), np.float64(1390.433845798219), np.float64(1394.290805148561), np.float64(1388.505366123048), np.float64(1396.219284823732)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(931.4556831075452), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(935.3126424578863), np.float64(956.5259188847667), np.float64(944.9550408337414), np.float64(937.2411221330576), np.float64(943.0265611585701), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(958.4543985599371), np.float64(1394.290805148561), np.float64(1392.36232547339), np.float64(1396.219284823732), np.float64(1390.433845798219)]</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[0.00582476 0.00518582 0.00501989 0.00493775 0.00482212 0.00474447
- 0.00466168 0.00457379 0.00445819 0.00444941 0.00440401 0.0044031
- 0.00436312 0.0043543  0.00431098 0.00428945 0.00427509 0.0042681
- 0.00419458 0.00418047]</t>
+          <t>[0.00635031 0.00574834 0.00563905 0.00553544 0.00544094 0.0052866
+ 0.00521664 0.00504912 0.00495718 0.0049308  0.00488007 0.00485697
+ 0.00479524 0.00477309 0.00475679 0.00433471 0.00422041 0.00420907
+ 0.00414546 0.00414229]</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>[0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277]</t>
+          <t>[0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356, 0.5269151138716356]</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -5018,10 +5018,10 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[0.00580431 0.00520319 0.00516744 0.0051339  0.00509628 0.00504794
- 0.00485087 0.00458955 0.00452306 0.00447026 0.00442417 0.00440461
- 0.00434644 0.0042466  0.00415649 0.00412601 0.00389114 0.00337637
- 0.00336886 0.00333457]</t>
+          <t>[0.00581209 0.00521065 0.00518234 0.00513964 0.00510274 0.005056
+ 0.00485618 0.0045937  0.00453101 0.00447434 0.00442779 0.00440824
+ 0.00435003 0.00424993 0.00415968 0.00412904 0.00389853 0.00338324
+ 0.00336778 0.00333313]</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -5088,20 +5088,20 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>[0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677, 0.546583850931677]</t>
+          <t>[0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435, 0.5348516218081435]</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[np.float64(1506.142626308473), np.float64(1508.071105983644), np.float64(1504.214146633302), np.float64(1509.999585658815), np.float64(1502.285666958131), np.float64(1511.928065333986), np.float64(1500.35718728296), np.float64(1513.856545009157), np.float64(1486.857829556764), np.float64(1484.929349881593), np.float64(1515.785024684327), np.float64(1488.786309231935), np.float64(1498.428707607789), np.float64(1490.714788907106), np.float64(1517.713504359498), np.float64(1496.500227932618), np.float64(1492.643268582277), np.float64(1483.000870206422), np.float64(1494.571748257448), np.float64(1519.641984034669)]</t>
+          <t>[np.float64(3050.854846120364), np.float64(929.5272034323739), np.float64(1704.776032851076), np.float64(1710.561471876588), np.float64(1706.704512526246), np.float64(1708.632992201417), np.float64(1600.638130391847), np.float64(1598.709650716676), np.float64(1602.566610067018), np.float64(1712.489951551759), np.float64(1700.919073500734), np.float64(1702.847553175905), np.float64(952.6689595344246), np.float64(1698.990593825563), np.float64(931.4556831075452), np.float64(1596.781171041505), np.float64(3048.926366445193), np.float64(950.7404798592538), np.float64(1604.495089742189), np.float64(954.5974392095954)]</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[0.00279142 0.00277976 0.00277577 0.00276157 0.00274253 0.00273489
- 0.00270479 0.00270251 0.00268797 0.00267181 0.00266765 0.00266722
- 0.00265615 0.00263139 0.00261845 0.00261756 0.00260333 0.00260199
- 0.00259952 0.00256077]</t>
+          <t>[0.00670334 0.0040861  0.00403634 0.00375772 0.00375351 0.00370002
+ 0.00345368 0.00341443 0.00331447 0.00328356 0.00327635 0.00323607
+ 0.00314673 0.00312925 0.00309629 0.00308285 0.00308135 0.00306802
+ 0.0030594  0.00298013]</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -5248,20 +5248,20 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>[0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277, 0.5189786059351277]</t>
+          <t>[0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505, 0.4939958592132505]</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[np.float64(929.5272034323739), np.float64(3050.854846120364), np.float64(952.6689595344246), np.float64(950.7404798592538), np.float64(954.5974392095954), np.float64(931.4556831075452), np.float64(948.812000184083), np.float64(956.5259188847667), np.float64(933.3841627827155), np.float64(946.8835205089117), np.float64(935.3126424578863), np.float64(937.2411221330576), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(944.9550408337414), np.float64(943.0265611585701), np.float64(958.4543985599371), np.float64(960.3828782351084), np.float64(1600.638130391847), np.float64(1515.785024684327)]</t>
+          <t>[np.float64(929.5272034323739), np.float64(952.6689595344246), np.float64(931.4556831075452), np.float64(950.7404798592538), np.float64(3050.854846120364), np.float64(954.5974392095954), np.float64(948.812000184083), np.float64(933.3841627827155), np.float64(956.5259188847667), np.float64(946.8835205089117), np.float64(935.3126424578863), np.float64(937.2411221330576), np.float64(939.1696018082284), np.float64(941.0980814833993), np.float64(944.9550408337414), np.float64(943.0265611585701), np.float64(958.4543985599371), np.float64(960.3828782351084), np.float64(1600.638130391847), np.float64(1602.566610067018)]</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>[0.00603269 0.00599442 0.00546726 0.00533677 0.0053211  0.00530717
- 0.00505471 0.00477765 0.00471855 0.00462611 0.0045492  0.00454175
- 0.00448936 0.00438218 0.00427711 0.00424554 0.00410928 0.00356187
- 0.00311393 0.00311379]</t>
+          <t>[0.00578676 0.00521034 0.00512719 0.0051078  0.00509916 0.00505039
+ 0.00487199 0.00459644 0.00451675 0.00449998 0.00443699 0.00441793
+ 0.00436149 0.00426937 0.00419026 0.00415766 0.00387923 0.00336621
+ 0.0032438  0.00319081]</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">

</xml_diff>